<commit_message>
pathology scores and models fitted
</commit_message>
<xml_diff>
--- a/data/pedagogic engagement/self-learning/Path Date - end of Initiation.xlsx
+++ b/data/pedagogic engagement/self-learning/Path Date - end of Initiation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grupolusofona-my.sharepoint.com/personal/a22204029_alunos_ulht_pt/Documents/Thesis - Sem 4/tumo-fdi-model/data/pedagogic engagement/self-learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0CDBB9D-1E09-4350-9888-D94270CD5309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{C0CDBB9D-1E09-4350-9888-D94270CD5309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27927C3C-0411-4E9E-A2EB-06452E727B93}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="26805" yWindow="4920" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -369,7 +369,7 @@
   <dimension ref="A1:F4398"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -379,7 +379,7 @@
     <col min="3" max="3" width="9.42578125" customWidth="1"/>
     <col min="4" max="4" width="4.140625" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>